<commit_message>
tz: improve the forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_2_child.xlsx
+++ b/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_2_child.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Tanzania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887E7357-C75C-46CB-9C83-1CDD76A66B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86BAF42-0E94-4D27-A1D1-52449C19C2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -123,9 +123,6 @@
     <t>. &gt;= 5 and . &lt;= 14</t>
   </si>
   <si>
-    <t>L’âge doit être compris entre 4 et 15 ans</t>
-  </si>
-  <si>
     <t>select_one sex</t>
   </si>
   <si>
@@ -493,6 +490,9 @@
   </si>
   <si>
     <t>Participants</t>
+  </si>
+  <si>
+    <t>Age must be between 4 and 15 years old</t>
   </si>
 </sst>
 </file>
@@ -1012,11 +1012,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1043,10 +1043,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>131</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>132</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>2</v>
@@ -1055,7 +1055,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>4</v>
@@ -1073,7 +1073,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1084,17 +1084,17 @@
         <v>9</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>129</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>130</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -1112,7 +1112,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="8"/>
@@ -1131,10 +1131,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="8"/>
@@ -1156,7 +1156,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="8"/>
@@ -1175,10 +1175,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="8"/>
@@ -1200,7 +1200,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="9"/>
@@ -1214,10 +1214,10 @@
     </row>
     <row r="8" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -1226,7 +1226,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -1234,13 +1234,13 @@
     </row>
     <row r="9" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>145</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>146</v>
       </c>
       <c r="D9" s="30"/>
       <c r="E9" s="29"/>
@@ -1254,10 +1254,10 @@
     </row>
     <row r="10" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -1266,7 +1266,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -1274,10 +1274,10 @@
     </row>
     <row r="11" spans="1:13" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -1286,7 +1286,7 @@
       <c r="G11" s="10"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -1300,10 +1300,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1321,21 +1321,21 @@
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>122</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>123</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
       <c r="F13" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9" t="s">
@@ -1344,27 +1344,27 @@
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:13" s="16" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="24"/>
       <c r="G14" s="10"/>
       <c r="H14" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>10</v>
@@ -1375,7 +1375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>20</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
@@ -1391,10 +1391,10 @@
         <v>22</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="9" t="s">
@@ -1405,20 +1405,20 @@
     </row>
     <row r="16" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="C16" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="21"/>
       <c r="H16" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="9" t="s">
@@ -1432,19 +1432,19 @@
         <v>18</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="21"/>
       <c r="H17" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="9" t="s">
@@ -1458,17 +1458,17 @@
         <v>18</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="21"/>
       <c r="H18" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="9" t="s">
@@ -1482,17 +1482,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="21"/>
       <c r="H19" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="9"/>
@@ -1504,17 +1504,17 @@
         <v>14</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="12"/>
       <c r="H20" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -1526,17 +1526,17 @@
         <v>14</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="12"/>
       <c r="H21" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -1548,10 +1548,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="11"/>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="31"/>
       <c r="C23" s="32"/>
@@ -1581,10 +1581,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>31</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>32</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="12"/>
@@ -1599,10 +1599,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>33</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>34</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="12"/>
@@ -1625,9 +1625,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G439"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1639,47 +1639,47 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1689,310 +1689,310 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="22" t="s">
-        <v>48</v>
-      </c>
       <c r="C30" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -4061,24 +4061,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>144</v>
-      </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tz: update sch/sth form
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_2_child.xlsx
+++ b/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_2_child.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Tanzania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF39DA3-B2EA-4C39-A73A-6A7BC8A9E1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A95A0A-B6D4-4DE9-8FE7-C712817B0E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="246">
   <si>
     <t>type</t>
   </si>
@@ -1336,11 +1336,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1617,9 @@
         <v>121</v>
       </c>
       <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="E9" s="24" t="s">
+        <v>121</v>
+      </c>
       <c r="F9" s="24"/>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -2288,7 +2290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D439"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>

</xml_diff>